<commit_message>
modified reference number in figures
</commit_message>
<xml_diff>
--- a/data_glutamate_09_04_2020.xlsx
+++ b/data_glutamate_09_04_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakobkaminski 1/glutamate_dlpfc_meta_repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543184BA-B77A-E74F-9099-52DD24F7BF90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2D72FA-3138-B147-BE82-0A6E811CFA67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8260" yWindow="460" windowWidth="20500" windowHeight="17500" xr2:uid="{DCE4E1A5-8D6D-F44F-BA21-78A407CE198F}"/>
   </bookViews>
@@ -612,7 +612,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -801,7 +801,7 @@
         <v>71</v>
       </c>
       <c r="S3">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="T3" t="s">
         <v>72</v>
@@ -863,7 +863,7 @@
         <v>71</v>
       </c>
       <c r="S4">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="T4" t="s">
         <v>72</v>
@@ -1297,7 +1297,7 @@
         <v>71</v>
       </c>
       <c r="S11">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="T11" t="s">
         <v>72</v>
@@ -1483,7 +1483,7 @@
         <v>71</v>
       </c>
       <c r="S14">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="T14" t="s">
         <v>72</v>

</xml_diff>